<commit_message>
Added full pipeline for screening drugs, working on pipeline for interactions
</commit_message>
<xml_diff>
--- a/data/beers.xlsx
+++ b/data/beers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ualbertaca-my.sharepoint.com/personal/hqiu1_ualberta_ca/Documents/Coding/BeersCriteria/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC021A9E-EF39-AC43-B9B5-3F31206BA734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{EC021A9E-EF39-AC43-B9B5-3F31206BA734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{113D896D-C9EC-41A4-918F-3ED1311775A8}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="10690" windowWidth="19420" windowHeight="10420" xr2:uid="{9320F0F9-4FE4-4246-8C0B-22926ED92CDD}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="16637" windowHeight="8837" firstSheet="2" activeTab="4" xr2:uid="{9320F0F9-4FE4-4246-8C0B-22926ED92CDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Avoid" sheetId="3" r:id="rId1"/>
@@ -2288,18 +2288,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D388D818-4AE7-4E44-B33A-C739097341D7}">
   <dimension ref="A1:C162"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="15.9" x14ac:dyDescent="0.9"/>
   <cols>
     <col min="1" max="1" width="27" style="1" customWidth="1"/>
     <col min="2" max="2" width="40" style="1" customWidth="1"/>
-    <col min="3" max="3" width="163.19921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="163.2109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A1" s="5" t="s">
         <v>212</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A10" s="5" t="s">
         <v>128</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="3" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" s="3" customFormat="1" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A13" s="5" t="s">
         <v>10</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A16" s="5" t="s">
         <v>13</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A17" s="5" t="s">
         <v>14</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A19" s="5" t="s">
         <v>16</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.9">
       <c r="A20" s="5" t="s">
         <v>17</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A21" s="5" t="s">
         <v>101</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A22" s="5" t="s">
         <v>19</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A23" s="5" t="s">
         <v>22</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A24" s="5" t="s">
         <v>105</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A25" s="5" t="s">
         <v>102</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A26" s="5" t="s">
         <v>103</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A27" s="5" t="s">
         <v>104</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A28" s="5" t="s">
         <v>18</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A29" s="5" t="s">
         <v>129</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A30" s="5" t="s">
         <v>20</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A31" s="5" t="s">
         <v>21</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A32" s="5" t="s">
         <v>344</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A33" s="5" t="s">
         <v>23</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A34" s="5" t="s">
         <v>348</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A35" s="5" t="s">
         <v>349</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A36" s="5" t="s">
         <v>347</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A37" s="5" t="s">
         <v>351</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A38" s="5" t="s">
         <v>24</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A39" s="5" t="s">
         <v>25</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A40" s="5" t="s">
         <v>26</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A41" s="5" t="s">
         <v>27</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A42" s="5" t="s">
         <v>28</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A43" s="5" t="s">
         <v>29</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="78" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="79.3" x14ac:dyDescent="0.9">
       <c r="A44" s="5" t="s">
         <v>342</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A45" s="5" t="s">
         <v>136</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A46" s="5" t="s">
         <v>30</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A47" s="5" t="s">
         <v>31</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A48" s="5" t="s">
         <v>32</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A49" s="5" t="s">
         <v>33</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A50" s="5" t="s">
         <v>34</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A51" s="5" t="s">
         <v>106</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A52" s="5" t="s">
         <v>35</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A53" s="5" t="s">
         <v>36</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A54" s="5" t="s">
         <v>37</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A55" s="5" t="s">
         <v>38</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A56" s="5" t="s">
         <v>39</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A57" s="5" t="s">
         <v>107</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A58" s="5" t="s">
         <v>108</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A59" s="5" t="s">
         <v>109</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A60" s="5" t="s">
         <v>110</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A61" s="5" t="s">
         <v>111</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A62" s="5" t="s">
         <v>112</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A63" s="5" t="s">
         <v>113</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A64" s="5" t="s">
         <v>114</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A65" s="5" t="s">
         <v>115</v>
       </c>
@@ -3014,7 +3014,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A66" s="5" t="s">
         <v>116</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A67" s="5" t="s">
         <v>117</v>
       </c>
@@ -3036,7 +3036,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A68" s="5" t="s">
         <v>118</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A69" s="5" t="s">
         <v>119</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A70" s="5" t="s">
         <v>120</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A71" s="5" t="s">
         <v>121</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A72" s="5" t="s">
         <v>122</v>
       </c>
@@ -3091,7 +3091,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A73" s="5" t="s">
         <v>123</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A74" s="5" t="s">
         <v>124</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A75" s="5" t="s">
         <v>125</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A76" s="5" t="s">
         <v>126</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A77" s="5" t="s">
         <v>127</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A78" s="5" t="s">
         <v>40</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A79" s="5" t="s">
         <v>41</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A80" s="5" t="s">
         <v>42</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A81" s="5" t="s">
         <v>43</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A82" s="5" t="s">
         <v>44</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A83" s="5" t="s">
         <v>45</v>
       </c>
@@ -3212,7 +3212,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A84" s="5" t="s">
         <v>46</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A85" s="5" t="s">
         <v>47</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A86" s="5" t="s">
         <v>48</v>
       </c>
@@ -3245,7 +3245,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A87" s="5" t="s">
         <v>49</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A88" s="5" t="s">
         <v>50</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A89" s="5" t="s">
         <v>51</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A90" s="5" t="s">
         <v>52</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A91" s="5" t="s">
         <v>135</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A92" s="5" t="s">
         <v>53</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A93" s="5" t="s">
         <v>54</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A94" s="5" t="s">
         <v>55</v>
       </c>
@@ -3333,7 +3333,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A95" s="5" t="s">
         <v>56</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A96" s="5" t="s">
         <v>57</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A97" s="5" t="s">
         <v>58</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A98" s="5" t="s">
         <v>352</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A99" s="5" t="s">
         <v>353</v>
       </c>
@@ -3388,7 +3388,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A100" s="5" t="s">
         <v>354</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A101" s="5" t="s">
         <v>53</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A102" s="5" t="s">
         <v>59</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A103" s="5" t="s">
         <v>60</v>
       </c>
@@ -3432,7 +3432,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A104" s="5" t="s">
         <v>61</v>
       </c>
@@ -3443,7 +3443,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A105" s="5" t="s">
         <v>62</v>
       </c>
@@ -3454,7 +3454,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A106" s="5" t="s">
         <v>63</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A107" s="5" t="s">
         <v>64</v>
       </c>
@@ -3476,7 +3476,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A108" s="5" t="s">
         <v>65</v>
       </c>
@@ -3487,7 +3487,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A109" s="5" t="s">
         <v>66</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A110" s="5" t="s">
         <v>355</v>
       </c>
@@ -3509,7 +3509,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A111" s="5" t="s">
         <v>356</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A112" s="5" t="s">
         <v>357</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A113" s="5" t="s">
         <v>358</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A114" s="5" t="s">
         <v>359</v>
       </c>
@@ -3553,7 +3553,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A115" s="5" t="s">
         <v>360</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A116" s="5" t="s">
         <v>361</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A117" s="5" t="s">
         <v>362</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A118" s="5" t="s">
         <v>363</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A119" s="5" t="s">
         <v>364</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A120" s="5" t="s">
         <v>366</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A121" s="5" t="s">
         <v>367</v>
       </c>
@@ -3630,7 +3630,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A122" s="5" t="s">
         <v>368</v>
       </c>
@@ -3641,7 +3641,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A123" s="5" t="s">
         <v>369</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A124" s="5" t="s">
         <v>67</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A125" s="5" t="s">
         <v>68</v>
       </c>
@@ -3674,7 +3674,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A126" s="5" t="s">
         <v>69</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A127" s="5" t="s">
         <v>130</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A128" s="5" t="s">
         <v>131</v>
       </c>
@@ -3707,7 +3707,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A129" s="5" t="s">
         <v>70</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A130" s="5" t="s">
         <v>132</v>
       </c>
@@ -3729,7 +3729,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" ht="126.9" x14ac:dyDescent="0.9">
       <c r="A131" s="5" t="s">
         <v>145</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" ht="126.9" x14ac:dyDescent="0.9">
       <c r="A132" s="5" t="s">
         <v>146</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" ht="126.9" x14ac:dyDescent="0.9">
       <c r="A133" s="5" t="s">
         <v>147</v>
       </c>
@@ -3762,7 +3762,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" ht="126.9" x14ac:dyDescent="0.9">
       <c r="A134" s="5" t="s">
         <v>148</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" ht="126.9" x14ac:dyDescent="0.9">
       <c r="A135" s="5" t="s">
         <v>149</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" ht="126.9" x14ac:dyDescent="0.9">
       <c r="A136" s="5" t="s">
         <v>150</v>
       </c>
@@ -3795,7 +3795,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A137" s="5" t="s">
         <v>71</v>
       </c>
@@ -3806,7 +3806,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A138" s="5" t="s">
         <v>133</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A139" s="5" t="s">
         <v>72</v>
       </c>
@@ -3828,7 +3828,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A140" s="5" t="s">
         <v>343</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A141" s="5" t="s">
         <v>73</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A142" s="5" t="s">
         <v>74</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A143" s="5" t="s">
         <v>75</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A144" s="5" t="s">
         <v>76</v>
       </c>
@@ -3883,7 +3883,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A145" s="5" t="s">
         <v>77</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A146" s="5" t="s">
         <v>370</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A147" s="5" t="s">
         <v>78</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A148" s="5" t="s">
         <v>79</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A149" s="5" t="s">
         <v>80</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A150" s="5" t="s">
         <v>81</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="151" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A151" s="5" t="s">
         <v>82</v>
       </c>
@@ -3960,7 +3960,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A152" s="5" t="s">
         <v>83</v>
       </c>
@@ -3971,7 +3971,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A153" s="5" t="s">
         <v>84</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A154" s="5" t="s">
         <v>85</v>
       </c>
@@ -3993,7 +3993,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A155" s="5" t="s">
         <v>134</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A156" s="5" t="s">
         <v>86</v>
       </c>
@@ -4015,7 +4015,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A157" s="5" t="s">
         <v>87</v>
       </c>
@@ -4026,7 +4026,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A158" s="5" t="s">
         <v>88</v>
       </c>
@@ -4037,7 +4037,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A159" s="5" t="s">
         <v>89</v>
       </c>
@@ -4048,7 +4048,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A160" s="5" t="s">
         <v>90</v>
       </c>
@@ -4059,7 +4059,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A161" s="5" t="s">
         <v>91</v>
       </c>
@@ -4070,7 +4070,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A162" s="5" t="s">
         <v>92</v>
       </c>
@@ -4093,19 +4093,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA6D8C55-7DA0-874E-81DC-96C4CB3816E2}">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A63" zoomScale="75" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="15.9" x14ac:dyDescent="0.9"/>
   <cols>
     <col min="1" max="1" width="30.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="69.296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.19921875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.796875" style="1"/>
+    <col min="2" max="2" width="69.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.2109375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.78515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A1" s="8" t="s">
         <v>212</v>
       </c>
@@ -4116,7 +4116,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="78" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="79.3" x14ac:dyDescent="0.9">
       <c r="A2" s="8" t="s">
         <v>380</v>
       </c>
@@ -4127,7 +4127,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A3" s="8" t="s">
         <v>93</v>
       </c>
@@ -4138,7 +4138,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A4" s="8" t="s">
         <v>94</v>
       </c>
@@ -4149,7 +4149,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A5" s="8" t="s">
         <v>95</v>
       </c>
@@ -4160,7 +4160,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A6" s="8" t="s">
         <v>107</v>
       </c>
@@ -4171,7 +4171,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A7" s="8" t="s">
         <v>108</v>
       </c>
@@ -4182,7 +4182,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A8" s="8" t="s">
         <v>109</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A9" s="8" t="s">
         <v>110</v>
       </c>
@@ -4204,7 +4204,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A10" s="8" t="s">
         <v>111</v>
       </c>
@@ -4215,7 +4215,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A11" s="8" t="s">
         <v>112</v>
       </c>
@@ -4226,7 +4226,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A12" s="8" t="s">
         <v>113</v>
       </c>
@@ -4237,7 +4237,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A13" s="8" t="s">
         <v>114</v>
       </c>
@@ -4248,7 +4248,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A14" s="8" t="s">
         <v>115</v>
       </c>
@@ -4259,7 +4259,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A15" s="8" t="s">
         <v>116</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A16" s="8" t="s">
         <v>117</v>
       </c>
@@ -4281,7 +4281,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A17" s="8" t="s">
         <v>118</v>
       </c>
@@ -4292,7 +4292,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A18" s="8" t="s">
         <v>119</v>
       </c>
@@ -4303,7 +4303,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A19" s="8" t="s">
         <v>120</v>
       </c>
@@ -4314,7 +4314,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A20" s="8" t="s">
         <v>121</v>
       </c>
@@ -4325,7 +4325,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A21" s="8" t="s">
         <v>122</v>
       </c>
@@ -4336,7 +4336,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A22" s="8" t="s">
         <v>123</v>
       </c>
@@ -4347,7 +4347,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A23" s="8" t="s">
         <v>124</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A24" s="8" t="s">
         <v>125</v>
       </c>
@@ -4369,7 +4369,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A25" s="8" t="s">
         <v>126</v>
       </c>
@@ -4380,7 +4380,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A26" s="8" t="s">
         <v>127</v>
       </c>
@@ -4391,7 +4391,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A27" s="8" t="s">
         <v>216</v>
       </c>
@@ -4402,7 +4402,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A28" s="8" t="s">
         <v>96</v>
       </c>
@@ -4413,7 +4413,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A29" s="9" t="s">
         <v>218</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A30" s="9" t="s">
         <v>219</v>
       </c>
@@ -4435,7 +4435,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A31" s="9" t="s">
         <v>220</v>
       </c>
@@ -4446,7 +4446,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A32" s="8" t="s">
         <v>221</v>
       </c>
@@ -4457,7 +4457,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A33" s="9" t="s">
         <v>222</v>
       </c>
@@ -4468,7 +4468,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A34" s="8" t="s">
         <v>217</v>
       </c>
@@ -4479,7 +4479,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A35" s="8" t="s">
         <v>223</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A36" s="8" t="s">
         <v>224</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A37" s="9" t="s">
         <v>225</v>
       </c>
@@ -4512,7 +4512,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A38" s="8" t="s">
         <v>226</v>
       </c>
@@ -4523,7 +4523,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A39" s="3" t="s">
         <v>381</v>
       </c>
@@ -4534,7 +4534,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A40" s="8" t="s">
         <v>227</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A41" s="8" t="s">
         <v>228</v>
       </c>
@@ -4556,7 +4556,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A42" s="8" t="s">
         <v>229</v>
       </c>
@@ -4567,7 +4567,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A43" s="8" t="s">
         <v>230</v>
       </c>
@@ -4578,7 +4578,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A44" s="8" t="s">
         <v>97</v>
       </c>
@@ -4589,7 +4589,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A45" s="8" t="s">
         <v>98</v>
       </c>
@@ -4600,7 +4600,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A46" s="8" t="s">
         <v>31</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A47" s="8" t="s">
         <v>32</v>
       </c>
@@ -4622,7 +4622,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A48" s="8" t="s">
         <v>33</v>
       </c>
@@ -4633,7 +4633,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A49" s="8" t="s">
         <v>34</v>
       </c>
@@ -4644,7 +4644,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A50" s="8" t="s">
         <v>231</v>
       </c>
@@ -4655,7 +4655,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A51" s="8" t="s">
         <v>35</v>
       </c>
@@ -4666,7 +4666,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A52" s="8" t="s">
         <v>36</v>
       </c>
@@ -4677,7 +4677,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A53" s="8" t="s">
         <v>37</v>
       </c>
@@ -4688,7 +4688,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A54" s="8" t="s">
         <v>38</v>
       </c>
@@ -4699,7 +4699,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A55" s="8" t="s">
         <v>39</v>
       </c>
@@ -4710,7 +4710,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A56" s="8" t="s">
         <v>232</v>
       </c>
@@ -4721,7 +4721,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A57" s="8" t="s">
         <v>233</v>
       </c>
@@ -4732,7 +4732,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A58" s="8" t="s">
         <v>234</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A59" s="8" t="s">
         <v>37</v>
       </c>
@@ -4754,7 +4754,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A60" s="8" t="s">
         <v>235</v>
       </c>
@@ -4765,7 +4765,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A61" s="8" t="s">
         <v>236</v>
       </c>
@@ -4776,7 +4776,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A62" s="8" t="s">
         <v>237</v>
       </c>
@@ -4787,7 +4787,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A63" s="8" t="s">
         <v>238</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A64" s="8" t="s">
         <v>239</v>
       </c>
@@ -4809,7 +4809,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A65" s="8" t="s">
         <v>240</v>
       </c>
@@ -4820,7 +4820,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A66" s="8" t="s">
         <v>99</v>
       </c>
@@ -4831,7 +4831,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A67" s="8" t="s">
         <v>382</v>
       </c>
@@ -4842,7 +4842,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A68" s="8" t="s">
         <v>100</v>
       </c>
@@ -4873,15 +4873,15 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="54" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="54" defaultRowHeight="15.9" x14ac:dyDescent="0.9"/>
   <cols>
     <col min="1" max="16384" width="54" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A1" s="4" t="s">
         <v>296</v>
       </c>
@@ -4895,7 +4895,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A2" s="8" t="s">
         <v>251</v>
       </c>
@@ -4909,7 +4909,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A3" s="8" t="s">
         <v>248</v>
       </c>
@@ -4923,7 +4923,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A4" s="8" t="s">
         <v>299</v>
       </c>
@@ -4937,7 +4937,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A5" s="8" t="s">
         <v>300</v>
       </c>
@@ -4951,7 +4951,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="47.6" x14ac:dyDescent="0.9">
       <c r="A6" s="8" t="s">
         <v>93</v>
       </c>
@@ -4965,7 +4965,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A7" s="8" t="s">
         <v>301</v>
       </c>
@@ -4979,7 +4979,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A8" s="8" t="s">
         <v>302</v>
       </c>
@@ -4993,7 +4993,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A9" s="8" t="s">
         <v>302</v>
       </c>
@@ -5007,7 +5007,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A10" s="8" t="s">
         <v>303</v>
       </c>
@@ -5021,7 +5021,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A11" s="8" t="s">
         <v>304</v>
       </c>
@@ -5035,7 +5035,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A12" s="8" t="s">
         <v>94</v>
       </c>
@@ -5049,7 +5049,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A13" s="8" t="s">
         <v>227</v>
       </c>
@@ -5063,7 +5063,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A14" s="8" t="s">
         <v>228</v>
       </c>
@@ -5077,7 +5077,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A15" s="8" t="s">
         <v>237</v>
       </c>
@@ -5091,7 +5091,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A16" s="8" t="s">
         <v>305</v>
       </c>
@@ -5105,7 +5105,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A17" s="8" t="s">
         <v>306</v>
       </c>
@@ -5119,7 +5119,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A18" s="8" t="s">
         <v>307</v>
       </c>
@@ -5133,7 +5133,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A19" s="8" t="s">
         <v>99</v>
       </c>
@@ -5147,7 +5147,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A20" s="8" t="s">
         <v>250</v>
       </c>
@@ -5161,7 +5161,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A21" s="8" t="s">
         <v>308</v>
       </c>
@@ -5175,7 +5175,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A22" s="8" t="s">
         <v>309</v>
       </c>
@@ -5189,7 +5189,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A23" s="8" t="s">
         <v>310</v>
       </c>
@@ -5203,7 +5203,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A24" s="8" t="s">
         <v>311</v>
       </c>
@@ -5217,7 +5217,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A25" s="8" t="s">
         <v>312</v>
       </c>
@@ -5244,19 +5244,19 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="15.9" x14ac:dyDescent="0.9"/>
   <cols>
-    <col min="1" max="1" width="27.19921875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="60.19921875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="34.296875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="61.796875" style="8" customWidth="1"/>
-    <col min="5" max="16384" width="10.796875" style="8"/>
+    <col min="1" max="1" width="27.2109375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="60.2109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="61.78515625" style="8" customWidth="1"/>
+    <col min="5" max="16384" width="10.78515625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A1" s="8" t="s">
         <v>184</v>
       </c>
@@ -5270,7 +5270,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A2" s="8" t="s">
         <v>187</v>
       </c>
@@ -5284,7 +5284,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A3" s="8" t="s">
         <v>186</v>
       </c>
@@ -5298,7 +5298,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A4" s="8" t="s">
         <v>272</v>
       </c>
@@ -5312,7 +5312,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A5" s="8" t="s">
         <v>271</v>
       </c>
@@ -5326,7 +5326,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="95.15" x14ac:dyDescent="0.9">
       <c r="A6" s="8" t="s">
         <v>189</v>
       </c>
@@ -5340,7 +5340,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="390" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="396.45" x14ac:dyDescent="0.9">
       <c r="A7" s="8" t="s">
         <v>191</v>
       </c>
@@ -5354,7 +5354,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="343.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="348.9" x14ac:dyDescent="0.9">
       <c r="A8" s="8" t="s">
         <v>192</v>
       </c>
@@ -5368,7 +5368,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="265.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="253.75" x14ac:dyDescent="0.9">
       <c r="A9" s="8" t="s">
         <v>193</v>
       </c>
@@ -5382,7 +5382,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="95.15" x14ac:dyDescent="0.9">
       <c r="A10" s="8" t="s">
         <v>194</v>
       </c>
@@ -5396,7 +5396,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A11" s="8" t="s">
         <v>195</v>
       </c>
@@ -5410,7 +5410,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A12" s="8" t="s">
         <v>196</v>
       </c>
@@ -5424,7 +5424,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A13" s="8" t="s">
         <v>390</v>
       </c>
@@ -5438,7 +5438,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="218.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="222" x14ac:dyDescent="0.9">
       <c r="A14" s="8" t="s">
         <v>389</v>
       </c>
@@ -5464,16 +5464,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC22E1C0-A1EE-7640-A114-DD751EA42CEA}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="32.2109375" defaultRowHeight="15.9" x14ac:dyDescent="0.9"/>
   <cols>
-    <col min="1" max="16384" width="32.19921875" style="1"/>
+    <col min="1" max="16384" width="32.2109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.9">
       <c r="A1" s="8" t="s">
         <v>243</v>
       </c>
@@ -5490,7 +5490,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="111" x14ac:dyDescent="0.9">
       <c r="A2" s="8" t="s">
         <v>259</v>
       </c>
@@ -5505,7 +5505,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="78" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="79.3" x14ac:dyDescent="0.9">
       <c r="A3" s="8" t="s">
         <v>261</v>
       </c>
@@ -5520,7 +5520,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="95.15" x14ac:dyDescent="0.9">
       <c r="A4" s="8" t="s">
         <v>261</v>
       </c>
@@ -5535,7 +5535,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.9">
       <c r="A5" s="8" t="s">
         <v>265</v>
       </c>
@@ -5550,7 +5550,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="409.5" x14ac:dyDescent="0.9">
       <c r="A6" s="8" t="s">
         <v>268</v>
       </c>
@@ -5567,7 +5567,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="111" x14ac:dyDescent="0.9">
       <c r="A7" s="8" t="s">
         <v>198</v>
       </c>
@@ -5582,7 +5582,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="63.45" x14ac:dyDescent="0.9">
       <c r="A8" s="8" t="s">
         <v>246</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A9" s="8" t="s">
         <v>246</v>
       </c>
@@ -5612,7 +5612,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A10" s="8" t="s">
         <v>275</v>
       </c>
@@ -5627,7 +5627,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.9">
       <c r="A11" s="8" t="s">
         <v>247</v>
       </c>
@@ -5642,7 +5642,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.9">
       <c r="A12" s="8" t="s">
         <v>249</v>
       </c>
@@ -5657,7 +5657,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.9">
       <c r="A13" s="8" t="s">
         <v>249</v>
       </c>
@@ -5672,7 +5672,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A14" s="8" t="s">
         <v>252</v>
       </c>
@@ -5687,7 +5687,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A15" s="8" t="s">
         <v>252</v>
       </c>
@@ -5702,7 +5702,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A16" s="8" t="s">
         <v>252</v>
       </c>
@@ -5717,7 +5717,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="31.75" x14ac:dyDescent="0.9">
       <c r="A17" s="8" t="s">
         <v>252</v>
       </c>
@@ -5732,7 +5732,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="111" x14ac:dyDescent="0.9">
       <c r="A18" s="8" t="s">
         <v>252</v>
       </c>

</xml_diff>